<commit_message>
updated when analysis to include ad-hoc and updated feedback
</commit_message>
<xml_diff>
--- a/when_test_controls_analysis_results.xlsx
+++ b/when_test_controls_analysis_results.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,16 +444,18 @@
   <cols>
     <col width="13.2" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
-    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="20.9" customWidth="1" min="3" max="3"/>
     <col width="20.9" customWidth="1" min="4" max="4"/>
-    <col width="19.8" customWidth="1" min="5" max="5"/>
+    <col width="26.4" customWidth="1" min="5" max="5"/>
     <col width="15.4" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="22" customWidth="1" min="8" max="8"/>
+    <col width="13.2" customWidth="1" min="8" max="8"/>
     <col width="22" customWidth="1" min="9" max="9"/>
     <col width="12.1" customWidth="1" min="10" max="10"/>
     <col width="22" customWidth="1" min="11" max="11"/>
     <col width="20.9" customWidth="1" min="12" max="12"/>
+    <col width="22" customWidth="1" min="13" max="13"/>
+    <col width="50" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -517,6 +519,16 @@
           <t>Multiple Controls</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Control Type Valid</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Control Type Message</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -526,20 +538,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The Audit Committee approves the exception reports daily to ensure compliance with internal policies.</t>
+          <t>Oracle Sub-Ledger Implementation Application is configured to accurately calculate depreciation entries from Oracle SL to Oracle GL</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>85.8</v>
+        <v>37.17810526315789</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Needs Improvement</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ESCALATION</t>
+          <t>WHEN, WHY, ESCALATION</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,16 +560,16 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>30</v>
+        <v>48.99999999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>28.8</v>
+        <v>67.18157894736841</v>
       </c>
       <c r="J2" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -567,6 +579,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate preventive</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -576,11 +598,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The Operations Team approves the user entitlements quarterly to ensure compliance with internal policies.</t>
+          <t>On an ad-hoc basis, The Data Access Management (DAM) team reviews the connections to ensure that they are operational to mitigate the risk of a missing connection that may lead to unauthorized access or sensitive data loss.</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>85.8</v>
+        <v>75.44999999999999</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -594,20 +616,20 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>may</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>30</v>
+        <v>79.99999999999999</v>
       </c>
       <c r="H3" t="n">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="I3" t="n">
-        <v>28.8</v>
+        <v>92.25</v>
       </c>
       <c r="J3" t="n">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -617,6 +639,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate automated</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -630,11 +662,11 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>74.31547058823529</v>
+        <v>89.51217882352941</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -648,16 +680,16 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H4" t="n">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="I4" t="n">
-        <v>17.31547058823529</v>
+        <v>86.91305882352941</v>
       </c>
       <c r="J4" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -667,6 +699,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate corrective</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -680,11 +722,11 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>71.09999999999999</v>
+        <v>75.92</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -698,23 +740,33 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>28.8</v>
+        <v>96</v>
       </c>
       <c r="J5" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K5" t="n">
-        <v>3.3</v>
+        <v>110</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate automated</t>
         </is>
       </c>
     </row>
@@ -730,7 +782,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>80.9316</v>
+        <v>93.42</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -748,16 +800,16 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H6" t="n">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="I6" t="n">
-        <v>23.9316</v>
+        <v>92.25</v>
       </c>
       <c r="J6" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -767,6 +819,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate preventive</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -780,16 +842,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>78.965</v>
+        <v>64.62</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ESCALATION</t>
+          <t>WHAT, ESCALATION</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -798,16 +860,16 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>30</v>
+        <v>89.99999999999999</v>
       </c>
       <c r="H7" t="n">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="I7" t="n">
-        <v>21.965</v>
+        <v>15</v>
       </c>
       <c r="J7" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -817,6 +879,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Control type in description (before) is consistent with preventive</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -830,7 +902,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>80.9316</v>
+        <v>88.02</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -848,16 +920,16 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>30</v>
+        <v>89.99999999999999</v>
       </c>
       <c r="H8" t="n">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="I8" t="n">
-        <v>23.9316</v>
+        <v>92.25</v>
       </c>
       <c r="J8" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -867,6 +939,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate detective</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -880,7 +962,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>65.39999999999999</v>
+        <v>62.22</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -898,16 +980,16 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>28.34999999999999</v>
+        <v>70</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>28.05</v>
+        <v>93.5</v>
       </c>
       <c r="J9" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -917,6 +999,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate detective</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -930,7 +1022,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>60.83920000000001</v>
+        <v>66.22</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -948,16 +1040,16 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>30</v>
+        <v>89.99999999999999</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>23.8392</v>
+        <v>92.25</v>
       </c>
       <c r="J10" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -967,6 +1059,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate corrective</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -980,7 +1082,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>65.8</v>
+        <v>65.81999999999999</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -998,16 +1100,16 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>30</v>
+        <v>84.99999999999999</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>28.8</v>
+        <v>96</v>
       </c>
       <c r="J11" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -1017,6 +1119,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate automated</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1030,7 +1142,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>57.26563</v>
+        <v>66.9665792</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1048,16 +1160,16 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>20.26563</v>
+        <v>84.58306</v>
       </c>
       <c r="J12" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
@@ -1067,6 +1179,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate preventive</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1080,7 +1202,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>85.8</v>
+        <v>87.61999999999999</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1098,16 +1220,16 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>30</v>
+        <v>84.99999999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="I13" t="n">
-        <v>28.8</v>
+        <v>96</v>
       </c>
       <c r="J13" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -1117,6 +1239,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate automated</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1130,16 +1262,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>63.17082352941176</v>
+        <v>89.02</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>WHEN, ESCALATION</t>
+          <t>ESCALATION</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1148,16 +1280,16 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I14" t="n">
-        <v>24.17082352941176</v>
+        <v>92.25</v>
       </c>
       <c r="J14" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -1167,6 +1299,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate corrective</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1180,7 +1322,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>71.09999999999999</v>
+        <v>72.72</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1198,23 +1340,33 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>30</v>
+        <v>89.99999999999999</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>28.8</v>
+        <v>96</v>
       </c>
       <c r="J15" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K15" t="n">
-        <v>3.3</v>
+        <v>110</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate corrective</t>
         </is>
       </c>
     </row>
@@ -1230,16 +1382,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>65.925</v>
+        <v>37.1</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Needs Improvement</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>WHEN, ESCALATION</t>
+          <t>WHEN, WHAT, ESCALATION</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1248,16 +1400,16 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>26.925</v>
+        <v>15</v>
       </c>
       <c r="J16" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
@@ -1267,6 +1419,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate automated</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1280,7 +1442,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>83.39999999999999</v>
+        <v>79.82000000000001</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1298,16 +1460,16 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>28.34999999999999</v>
+        <v>70</v>
       </c>
       <c r="H17" t="n">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="I17" t="n">
-        <v>28.05</v>
+        <v>93.5</v>
       </c>
       <c r="J17" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K17" t="n">
         <v>0</v>
@@ -1317,6 +1479,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate detective</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1330,16 +1502,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>46.56547058823529</v>
+        <v>87.31217882352941</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Needs Improvement</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>WHEN, ESCALATION</t>
+          <t>ESCALATION</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1348,16 +1520,16 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>20.25</v>
+        <v>100</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I18" t="n">
-        <v>17.31547058823529</v>
+        <v>86.91305882352941</v>
       </c>
       <c r="J18" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
@@ -1367,6 +1539,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate detective</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1380,16 +1562,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>67.8</v>
+        <v>43.5</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Needs Improvement</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>WHEN, ESCALATION</t>
+          <t>WHEN, WHAT, ESCALATION</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1398,16 +1580,16 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>30</v>
+        <v>89.99999999999999</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>28.8</v>
+        <v>15</v>
       </c>
       <c r="J19" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
@@ -1417,6 +1599,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate corrective</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1430,7 +1622,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>71.09999999999999</v>
+        <v>72.72</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1448,23 +1640,33 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>30</v>
+        <v>89.99999999999999</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>28.8</v>
+        <v>96</v>
       </c>
       <c r="J20" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K20" t="n">
-        <v>3.3</v>
+        <v>110</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate corrective</t>
         </is>
       </c>
     </row>
@@ -1480,7 +1682,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>65.05</v>
+        <v>60.22</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1498,16 +1700,16 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>28.05</v>
+        <v>93.5</v>
       </c>
       <c r="J21" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
@@ -1517,6 +1719,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate corrective</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1530,7 +1742,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>79.59999999999999</v>
+        <v>81.604</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1548,16 +1760,16 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>28.34999999999999</v>
+        <v>70</v>
       </c>
       <c r="H22" t="n">
-        <v>16.2</v>
+        <v>97.2</v>
       </c>
       <c r="I22" t="n">
-        <v>28.05</v>
+        <v>93.5</v>
       </c>
       <c r="J22" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K22" t="n">
         <v>0</v>
@@ -1567,6 +1779,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate preventive</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1580,7 +1802,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>65.39999999999999</v>
+        <v>59.98</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1598,16 +1820,16 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>28.34999999999999</v>
+        <v>62.99999999999999</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>28.05</v>
+        <v>93.5</v>
       </c>
       <c r="J23" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K23" t="n">
         <v>0</v>
@@ -1617,6 +1839,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate detective</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1630,7 +1862,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>85.8</v>
+        <v>92.42</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1648,16 +1880,16 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H24" t="n">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="I24" t="n">
-        <v>28.8</v>
+        <v>96</v>
       </c>
       <c r="J24" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K24" t="n">
         <v>0</v>
@@ -1667,6 +1899,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate automated</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1680,7 +1922,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>63.816</v>
+        <v>71.42</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1698,16 +1940,16 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>24.816</v>
+        <v>92.25</v>
       </c>
       <c r="J25" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K25" t="n">
         <v>0</v>
@@ -1717,6 +1959,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate detective</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1730,11 +1982,11 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>63.13652631578947</v>
+        <v>78.69997473684211</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1748,16 +2000,16 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>20.25</v>
+        <v>70</v>
       </c>
       <c r="H26" t="n">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="I26" t="n">
-        <v>16.88652631578947</v>
+        <v>86.56242105263158</v>
       </c>
       <c r="J26" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K26" t="n">
         <v>0</v>
@@ -1767,6 +2019,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate automated</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1780,7 +2042,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>67.8</v>
+        <v>69.42</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1798,16 +2060,16 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>30</v>
+        <v>89.99999999999999</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>28.8</v>
+        <v>96</v>
       </c>
       <c r="J27" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K27" t="n">
         <v>0</v>
@@ -1817,6 +2079,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate detective</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1830,7 +2102,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>66.45269999999999</v>
+        <v>74.72</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1848,23 +2120,33 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>24.1527</v>
+        <v>92.25</v>
       </c>
       <c r="J28" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K28" t="n">
-        <v>3.3</v>
+        <v>110</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate detective</t>
         </is>
       </c>
     </row>
@@ -1880,7 +2162,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>68.69999999999999</v>
+        <v>58.8</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1898,23 +2180,33 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>28.34999999999999</v>
+        <v>48.99999999999999</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>28.05</v>
+        <v>93.5</v>
       </c>
       <c r="J29" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K29" t="n">
-        <v>3.3</v>
+        <v>110</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate automated</t>
         </is>
       </c>
     </row>
@@ -1930,16 +2222,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>83.925</v>
+        <v>66.5</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>ESCALATION</t>
+          <t>WHAT, ESCALATION</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1948,16 +2240,16 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H30" t="n">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="I30" t="n">
-        <v>26.925</v>
+        <v>15</v>
       </c>
       <c r="J30" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K30" t="n">
         <v>0</v>
@@ -1967,6 +2259,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate detective</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1980,7 +2282,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>84</v>
+        <v>87.23999999999999</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1998,16 +2300,16 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>30</v>
+        <v>89.99999999999999</v>
       </c>
       <c r="H31" t="n">
-        <v>16.2</v>
+        <v>81</v>
       </c>
       <c r="I31" t="n">
-        <v>28.8</v>
+        <v>96</v>
       </c>
       <c r="J31" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="K31" t="n">
         <v>0</v>
@@ -2015,6 +2317,16 @@
       <c r="L31" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>Control type in description does not indicate automated</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2350,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.2" customWidth="1" min="1" max="1"/>
-    <col width="35.2" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
     <col width="31.9" customWidth="1" min="3" max="3"/>
     <col width="50" customWidth="1" min="4" max="4"/>
     <col width="50" customWidth="1" min="5" max="5"/>
@@ -2085,22 +2397,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The Audit Committee</t>
+          <t>Oracle Sub-Ledger Implementation Application</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>daily</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>approves the exception reports daily to ensure compliance with internal policies</t>
+          <t>calculate depreciation entries from oracle sl to oracle</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Audit Committee approves the exception reports daily to ensure compliance with internal policies., The Audit Committee approves the exception reports daily to ensure compliance with internal policies.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2117,22 +2429,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The Operations Team</t>
+          <t>The Data Access Management (DAM) team</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>quarterly</t>
+          <t>on an ad-hoc basis</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>approves the user entitlements</t>
+          <t>reviews the connections</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Operations Team approves the user entitlements quarterly to ensure compliance with internal policies., The Operations Team approves the user entitlements quarterly to ensure compliance with internal policies.</t>
+          <t xml:space="preserve">to ensure that they are operational to mitigate the risk of </t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2164,7 +2476,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Operations Team monitors the monthly reconciliations within defined timelines to ensure compliance with internal policies., The Operations Team monitors the monthly reconciliations within defined timelines to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -2196,7 +2508,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Operations Team reconciles the financial reports to ensure compliance with internal policies., The Operations Team reconciles the financial reports to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2228,7 +2540,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Compliance Officer reviews the monthly reconciliations to ensure compliance with internal policies., The Compliance Officer reviews the monthly reconciliations to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -2255,12 +2567,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>reviews</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The IT Administrator reviews the access logs before each financial close to ensure compliance with internal policies., The IT Administrator reviews the access logs before each financial close to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2292,7 +2604,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The IT Administrator reviews the monthly reconciliations to ensure compliance with internal policies., The IT Administrator reviews the monthly reconciliations to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2324,7 +2636,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Operations Team tests the user entitlements to ensure compliance with internal policies., The Operations Team tests the user entitlements to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2356,7 +2668,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Risk Management Department reviews the risk assessments periodically to ensure compliance with internal policies., The Risk Management Department reviews the risk assessments periodically to ensure compliance with internal policies., The Risk Management Department reviews the risk assessments periodically to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -2388,7 +2700,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Audit Committee reconciles the user entitlements periodically to ensure compliance with internal policies., The Audit Committee reconciles the user entitlements periodically to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -2415,12 +2727,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>reviews the financial reports when appropriate to ensure compliance with internal policies</t>
+          <t>reviews the financial reports</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Accounting Manager reviews the financial reports when appropriate to ensure compliance with internal policies., The Accounting Manager reviews the financial reports when appropriate to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -2452,7 +2764,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Audit Committee reconciles the exception reports every Friday to ensure compliance with internal policies., The Audit Committee reconciles the exception reports every Friday to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -2474,7 +2786,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>within defined timelines to</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2484,7 +2796,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Operations Team reviews the financial reports within defined timelines to ensure compliance with internal policies., The Operations Team reviews the financial reports within defined timelines to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2516,7 +2828,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Risk Management Department approves the financial reports to ensure compliance with internal policies., The Risk Management Department approves the financial reports to ensure compliance with internal policies., The Risk Management Department approves the financial reports to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2543,12 +2855,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>validates the exception reports according to procedure to ensure compliance with internal policies</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The IT Administrator validates the exception reports according to procedure to ensure compliance with internal policies., The IT Administrator validates the exception reports according to procedure to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2575,12 +2887,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>tests the financial reports before each financial close</t>
+          <t>tests the financial reports</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Audit Committee tests the financial reports before each financial close to ensure compliance with internal policies., The Audit Committee tests the financial reports before each financial close to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2602,7 +2914,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>within defined timelines to</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2612,7 +2924,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Audit Committee monitors the risk assessments within defined timelines to ensure compliance with internal policies., The Audit Committee monitors the risk assessments within defined timelines to ensure compliance with internal policies., The Audit Committee monitors the risk assessments within defined timelines to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2639,12 +2951,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>approves</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The IT Administrator approves the access logs from time to time to ensure compliance with internal policies., The IT Administrator approves the access logs from time to time to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2676,7 +2988,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The IT Administrator validates the exception reports to ensure compliance with internal policies., The IT Administrator validates the exception reports to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2708,7 +3020,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Compliance Officer tests the user entitlements periodically to ensure compliance with internal policies., The Compliance Officer tests the user entitlements periodically to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2740,7 +3052,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Audit Committee tests the monthly reconciliations regularly to ensure compliance with internal policies., The Audit Committee tests the monthly reconciliations regularly to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2772,7 +3084,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Risk Management Department tests the risk assessments to ensure compliance with internal policies., The Risk Management Department tests the risk assessments to ensure compliance with internal policies., The Risk Management Department tests the risk assessments to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2804,7 +3116,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Operations Team approves the risk assessments quarterly to ensure compliance with internal policies., The Operations Team approves the risk assessments quarterly to ensure compliance with internal policies., The Operations Team approves the risk assessments quarterly to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2836,7 +3148,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Compliance Officer reviews the access logs to ensure compliance with internal policies., The Compliance Officer reviews the access logs to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2868,7 +3180,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Risk Management Department monitors the risk assessments within 3 business days to ensure compliance with internal policies., The Risk Management Department monitors the risk assessments within 3 business days to ensure compliance with internal policies., The Risk Management Department monitors the risk assessments within 3 business days to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2900,7 +3212,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The IT Administrator reconciles the risk assessments to ensure compliance with internal policies., The IT Administrator reconciles the risk assessments to ensure compliance with internal policies., The IT Administrator reconciles the risk assessments to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2932,7 +3244,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Audit Committee reviews the exception reports to ensure compliance with internal policies., The Audit Committee reviews the exception reports to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2964,7 +3276,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Risk Management Department tests the financial reports to ensure compliance with internal policies., The Risk Management Department tests the financial reports to ensure compliance with internal policies., The Risk Management Department tests the financial reports to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2991,12 +3303,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>reconciles</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Operations Team reconciles the access logs annually to ensure compliance with internal policies., The Operations Team reconciles the access logs annually to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3028,7 +3340,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>to ensure compliance with internal policies, The Compliance Officer reconciles the monthly reconciliations from time to time to ensure compliance with internal policies., The Compliance Officer reconciles the monthly reconciliations from time to time to ensure compliance with internal policies.</t>
+          <t>to ensure compliance with internal policies</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3057,10 +3369,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.2" customWidth="1" min="1" max="1"/>
-    <col width="15.4" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
     <col width="50" customWidth="1" min="4" max="4"/>
-    <col width="50" customWidth="1" min="5" max="5"/>
+    <col width="15.4" customWidth="1" min="5" max="5"/>
     <col width="50" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -3102,31 +3414,23 @@
           <t>TEST-1000</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Consider using active voice to clearly indicate responsibility for control activities.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Control mentions exceptions but doesn't specify how they are handled or escalated</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -3136,29 +3440,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Warning: Human performer detected for automated control</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>While 'ad-hoc' is an allowed frequency, the control would be stronger if it specified what triggers the ad-hoc review.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Consider clarifying the object of 'review' to be more specific.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -3166,31 +3466,15 @@
           <t>TEST-1002</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Replace weak verb 'monitors' with a stronger control verb like 'track', 'supervise', or 'observe'</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3200,7 +3484,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Warning: Human performer detected for automated control</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3208,21 +3492,13 @@
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -3230,31 +3506,15 @@
           <t>TEST-1004</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -3262,31 +3522,19 @@
           <t>TEST-1005</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Consider clarifying the object of 'review' to be more specific.</t>
+          <t>No clear control action detected; add a specific verb describing what the control does</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -3294,31 +3542,15 @@
           <t>TEST-1006</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -3326,31 +3558,19 @@
           <t>TEST-1007</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3358,31 +3578,19 @@
           <t>TEST-1008</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Replace vague timing term 'periodically' with specific frequency (daily, weekly, monthly).</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3392,7 +3600,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Warning: Human performer detected for automated control</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -3400,21 +3608,13 @@
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Replace vague timing term 'periodically' with specific frequency (daily, weekly, monthly).</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3422,31 +3622,19 @@
           <t>TEST-1010</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Replace vague timing term 'when appropriate' with specific criteria for when the control is appropriate.</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3456,14 +3644,10 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>Warning: Human performer detected for automated control</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
           <t>Consider clarifying the object of 'reconcile' to be more specific.</t>
@@ -3471,7 +3655,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -3486,31 +3670,15 @@
           <t>TEST-1012</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3518,31 +3686,19 @@
           <t>TEST-1013</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3552,7 +3708,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Warning: Human performer detected for automated control</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -3562,12 +3718,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Consider clarifying the object of 'validate' to be more specific.</t>
+          <t>No clear control action detected; add a specific verb describing what the control does</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -3582,31 +3738,15 @@
           <t>TEST-1015</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3614,31 +3754,15 @@
           <t>TEST-1016</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Replace weak verb 'monitors' with a stronger control verb like 'track', 'supervise', or 'observe'</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3646,11 +3770,7 @@
           <t>TEST-1017</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Replace vague timing term 'from time to time' with specific frequency or conditions.</t>
@@ -3658,19 +3778,15 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Consider clarifying the object of 'approve' to be more specific.</t>
+          <t>No clear control action detected; add a specific verb describing what the control does</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3678,31 +3794,19 @@
           <t>TEST-1018</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3710,31 +3814,19 @@
           <t>TEST-1019</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).; Replace vague timing term 'periodically' with specific frequency (daily, weekly, monthly).</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3742,31 +3834,19 @@
           <t>TEST-1020</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
           <t>Replace vague timing term 'regularly' with specific frequency (daily, weekly, monthly).</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3774,31 +3854,19 @@
           <t>TEST-1021</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3808,29 +3876,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>Warning: Human performer detected for automated control</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3838,31 +3894,19 @@
           <t>TEST-1023</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3872,29 +3916,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Replace weak verb 'monitors' with a stronger control verb like 'track', 'supervise', or 'observe'</t>
-        </is>
-      </c>
+          <t>Warning: Human performer detected for automated control</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3902,31 +3934,19 @@
           <t>TEST-1025</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3934,31 +3954,19 @@
           <t>TEST-1026</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3968,7 +3976,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Warning: Human performer detected for automated control</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -3976,21 +3984,13 @@
           <t>No specific timing information detected. Add specific frequency (daily, weekly, monthly) or timing (within X days).</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3998,31 +3998,19 @@
           <t>TEST-1028</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Consider clarifying the object of 'reconcile' to be more specific.</t>
+          <t>No clear control action detected; add a specific verb describing what the control does</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4032,7 +4020,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Warning: Human performer detected for automated control</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -4040,21 +4028,13 @@
           <t>Replace vague timing term 'from time to time' with specific frequency or conditions.</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Control has a WHY statement focused on compliance. Consider specifying which regulations or policies this control supports.</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4067,7 +4047,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4132,7 +4112,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -4142,7 +4122,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -4152,7 +4132,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -4201,7 +4181,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17 (56.7%)</t>
+          <t>16 (53.3%)</t>
         </is>
       </c>
     </row>
@@ -4213,7 +4193,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0 (0.0%)</t>
+          <t>4 (13.3%)</t>
         </is>
       </c>
     </row>
@@ -4225,7 +4205,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0 (0.0%)</t>
+          <t>1 (3.3%)</t>
         </is>
       </c>
     </row>
@@ -4246,7 +4226,7 @@
       <c r="B19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Top Vague Terms</t>
         </is>
@@ -4268,7 +4248,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>appropriate</t>
+          <t>may</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4280,12 +4260,60 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>appropriate</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1 (3.3%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>regularly</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>1 (3.3%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Control Type Validation</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Valid Control Type</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1 (3.3%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Invalid Control Type</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>29 (96.7%)</t>
         </is>
       </c>
     </row>
@@ -4300,7 +4328,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4335,7 +4363,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>This analysis evaluates control descriptions based on seven key elements that should be present in a well-written control description:</t>
+          <t>This analysis evaluates control descriptions based on five key elements that should be present in a well-written control description:</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -4483,7 +4511,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>WHO: 30%</t>
+          <t>WHO: 32%</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -4491,7 +4519,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>WHEN: 20%</t>
+          <t>WHEN: 22%</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -4499,7 +4527,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>WHAT: 30%</t>
+          <t>WHAT: 32%</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -4507,7 +4535,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>WHY: 10%</t>
+          <t>WHY: 11%</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -4595,6 +4623,46 @@
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Enhanced Validation Checks</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Control Type Validation:</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Validates consistency between control actions and declared control type.</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Provides context-specific feedback for preventive, detective, corrective, and automated controls.</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>